<commit_message>
formatos vacios de cambios de rquerimiento
</commit_message>
<xml_diff>
--- a/Entregable 1/Nomenclaturas.xlsx
+++ b/Entregable 1/Nomenclaturas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank\Desktop\Incidencias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Desarrollo 2\Documentacion\Entregable 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1092,7 +1092,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>36</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
@@ -1462,7 +1462,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se elimino carpeta de canvas
</commit_message>
<xml_diff>
--- a/Entregable 1/Nomenclaturas.xlsx
+++ b/Entregable 1/Nomenclaturas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6465" windowHeight="3420" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="6465" windowHeight="3420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1462,7 +1462,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>